<commit_message>
rerun mode choice for nonGerman cities
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/carown_LR/All_short_edit_carown.xlsx
+++ b/outputs/ML_Results/carown_LR/All_short_edit_carown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\projects\sufficcs_mobility\outputs\ML_Results\carown_LR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{39716405-1470-4061-8334-3223E442520F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10AA18A-B473-465E-BB75-D434345D7179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All_short" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All_short!$A$1:$D$69</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -170,10 +183,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -660,13 +674,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1043,7 +1060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D69"/>
   <sheetViews>
@@ -1939,7 +1956,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D69">
+  <autoFilter ref="A1:D69" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="bike_lane_share"/>
@@ -1959,11 +1976,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:F19"/>
+      <selection activeCell="E3" sqref="E3:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2004,16 +2021,16 @@
         <v>45</v>
       </c>
       <c r="C3" s="4">
-        <v>2.8965458034299998E-4</v>
+        <v>3.87898767509E-4</v>
       </c>
       <c r="D3" s="4">
-        <v>6.2554905993570005E-4</v>
+        <v>6.2511732449640003E-4</v>
       </c>
       <c r="E3" s="4">
-        <v>8.9025158882620004E-4</v>
+        <v>9.0422719854750002E-4</v>
       </c>
       <c r="F3" s="4">
-        <v>2.9382142633410001E-4</v>
+        <v>4.9687461771749999E-4</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -2030,16 +2047,16 @@
         <v>46</v>
       </c>
       <c r="C5" s="3">
-        <v>1.9655401788143401E-2</v>
+        <v>2.2854772359507999E-2</v>
       </c>
       <c r="D5" s="3">
-        <v>1.49000958172118E-2</v>
+        <v>1.4818344266720299E-2</v>
       </c>
       <c r="E5" s="3">
-        <v>-8.9012174126317997E-3</v>
+        <v>-9.3540856976506992E-3</v>
       </c>
       <c r="F5" s="3">
-        <v>6.6725116001821998E-3</v>
+        <v>8.1783064607498998E-3</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -2047,23 +2064,27 @@
         <v>29</v>
       </c>
       <c r="C6" s="3">
-        <v>-0.1859657742185</v>
+        <v>-0.20116805500895499</v>
       </c>
       <c r="D6" s="3">
-        <v>0.28055750134426899</v>
+        <v>0.28020287174260899</v>
       </c>
       <c r="E6" s="3">
-        <v>0.62977771214283396</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>0.61830414749449203</v>
+      </c>
+      <c r="F6" s="6">
+        <v>-0.144916400383516</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3">
+        <v>0.21905184873164901</v>
+      </c>
       <c r="D7" s="6">
-        <v>0.25834518080476698</v>
+        <v>0.268627788752136</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2073,13 +2094,13 @@
         <v>31</v>
       </c>
       <c r="C8" s="3">
-        <v>-1.15873770786592</v>
+        <v>-1.1411954057353699</v>
       </c>
       <c r="D8" s="3">
-        <v>-0.59598908219801705</v>
+        <v>-0.60701799021159697</v>
       </c>
       <c r="E8" s="3">
-        <v>-0.93907657745742401</v>
+        <v>-0.94270408428858499</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -2088,13 +2109,13 @@
         <v>32</v>
       </c>
       <c r="C9" s="3">
-        <v>-0.73048603589795202</v>
+        <v>-0.60202951047286002</v>
       </c>
       <c r="D9" s="3">
-        <v>-0.36446380620935798</v>
+        <v>-0.36902068625568901</v>
       </c>
       <c r="E9" s="3">
-        <v>-0.77324117745895504</v>
+        <v>-0.77526779572538196</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -2103,13 +2124,13 @@
         <v>33</v>
       </c>
       <c r="C10" s="6">
-        <v>-0.196570447257155</v>
+        <v>-0.19620411180945799</v>
       </c>
       <c r="D10" s="3">
-        <v>-0.37763417564768198</v>
+        <v>-0.37725997561816299</v>
       </c>
       <c r="E10" s="3">
-        <v>-0.920039240166453</v>
+        <v>-0.92837803545025499</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -2118,16 +2139,16 @@
         <v>34</v>
       </c>
       <c r="C11" s="3">
-        <v>7.4401019838715304E-2</v>
+        <v>8.9352333545230894E-2</v>
       </c>
       <c r="D11" s="3">
-        <v>4.5423157188550799E-2</v>
+        <v>5.8491475457904202E-2</v>
       </c>
       <c r="E11" s="3">
-        <v>4.3658074406936802E-2</v>
+        <v>5.2762775345620003E-2</v>
       </c>
       <c r="F11" s="3">
-        <v>6.5271015942206106E-2</v>
+        <v>8.9356414656360295E-2</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -2144,14 +2165,16 @@
         <v>36</v>
       </c>
       <c r="C13" s="4">
-        <v>-7.1661348124692502E-5</v>
-      </c>
-      <c r="D13" s="4">
-        <v>-2.8738707745520899E-5</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4">
-        <v>-5.0163706749011102E-5</v>
+        <v>-8.2830891356175195E-5</v>
+      </c>
+      <c r="D13" s="8">
+        <v>-2.66765633695503E-5</v>
+      </c>
+      <c r="E13" s="9">
+        <v>-6.2106967298805499E-5</v>
+      </c>
+      <c r="F13" s="8">
+        <v>-4.7534825517733303E-5</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
@@ -2161,31 +2184,28 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3">
-        <f>1000000*-3.56353059744719E-08</f>
-        <v>-3.5635305974471905E-2</v>
-      </c>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="6">
-        <v>-6.6118888595850999E-3</v>
-      </c>
-      <c r="E15" s="6">
-        <v>-6.5442954325590002E-3</v>
-      </c>
-      <c r="F15" s="3"/>
+      <c r="D15" s="7">
+        <v>-8.1030419149614001E-3</v>
+      </c>
+      <c r="E15" s="7">
+        <v>-7.0797778685479998E-3</v>
+      </c>
+      <c r="F15" s="3">
+        <v>-8.7100682453192992E-3</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="6">
-        <v>2.7696001435435998E-3</v>
-      </c>
+      <c r="C16" s="6"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2196,13 +2216,13 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3">
-        <v>-2.1087185295746401E-2</v>
+        <v>-2.1921995511493E-2</v>
       </c>
       <c r="E17" s="3">
-        <v>-1.9654417123701699E-2</v>
+        <v>-1.5486784672823E-2</v>
       </c>
       <c r="F17" s="3">
-        <v>-1.4055178883940801E-2</v>
+        <v>-1.54305993326835E-2</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -2214,17 +2234,15 @@
         <v>41</v>
       </c>
       <c r="C18" s="3">
-        <v>1.1972076867557101E-2</v>
+        <v>1.0528781781078401E-2</v>
       </c>
       <c r="D18" s="3">
-        <v>1.19279696770729E-2</v>
-      </c>
-      <c r="E18" s="3">
-        <v>3.9187226468170397E-2</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1.5880564946568702E-2</v>
-      </c>
+        <v>8.0116596672203996E-3</v>
+      </c>
+      <c r="E18" s="6">
+        <v>7.4460871814086803E-3</v>
+      </c>
+      <c r="F18" s="3"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -2234,14 +2252,12 @@
       <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="3">
+        <v>-5.9616654342487304E-3</v>
+      </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3">
-        <v>3.4537416681146599E-2</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1.2822334510362E-2</v>
-      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>

</xml_diff>